<commit_message>
[FEATURE] Se agrego script y funcionalidad para COMPENSACION COELSA
</commit_message>
<xml_diff>
--- a/Test Data/Compensacion Coelsa.xlsx
+++ b/Test Data/Compensacion Coelsa.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo.Ameztoy\git\Crecer\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{AF9F1DA1-1816-4953-B9EC-40163DFA7738}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
+  <xr:revisionPtr documentId="13_ncr:1_{039BAF99-2216-43F9-ADA9-C1E80C57EDBA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
     <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="IDS" r:id="rId1" sheetId="2"/>
-    <sheet name="Hoja1" r:id="rId2" sheetId="1"/>
-    <sheet name="Hoja2" r:id="rId3" sheetId="3"/>
+    <sheet name="numOPER" r:id="rId1" sheetId="4"/>
+    <sheet name="IDS" r:id="rId2" sheetId="2"/>
+    <sheet name="Hoja1" r:id="rId3" sheetId="1"/>
+    <sheet name="Hoja2" r:id="rId4" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>ID COELSA</t>
   </si>
@@ -107,31 +108,31 @@
     <t>01372</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>FT23023100445860</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>ARS1535900011242</t>
-  </si>
-  <si>
-    <t>02425987087</t>
-  </si>
-  <si>
-    <t>550,00</t>
-  </si>
-  <si>
-    <t>IMP</t>
-  </si>
-  <si>
-    <t>20650</t>
-  </si>
-  <si>
-    <t>07050</t>
+    <t>33270660</t>
+  </si>
+  <si>
+    <t>FT23025851695505</t>
+  </si>
+  <si>
+    <t>INSTITUTO HIJAS DE MARIA SANTISIMA</t>
+  </si>
+  <si>
+    <t>ARS1535900011001</t>
+  </si>
+  <si>
+    <t>10010082298</t>
+  </si>
+  <si>
+    <t>100,00</t>
+  </si>
+  <si>
+    <t>30507126509</t>
+  </si>
+  <si>
+    <t>20170754337</t>
+  </si>
+  <si>
+    <t>30507126509-VAR-INSTITUTO HIJAS DE MARI</t>
   </si>
 </sst>
 </file>
@@ -458,10 +459,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6BA4F8-204C-431E-B085-9923979E146E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>33270660</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE588A77-7916-456E-8842-4629CC4FE9A4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -484,9 +511,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -496,11 +523,12 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="33.7109375" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
@@ -583,153 +611,39 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -739,7 +653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319500D4-7A0E-4018-92DB-C1A7EFAD4314}">
   <dimension ref="A1:N1"/>
   <sheetViews>

</xml_diff>